<commit_message>
Tabela de tradução NCMxCNAE
</commit_message>
<xml_diff>
--- a/Tabela de correspondencia CNAE x NCM_v4.xlsx
+++ b/Tabela de correspondencia CNAE x NCM_v4.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6114" uniqueCount="4667">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6114" uniqueCount="4669">
   <si>
     <t>NCM_descricao</t>
   </si>
@@ -14022,6 +14022,12 @@
   </si>
   <si>
     <t>NCM_2011_e_atuais</t>
+  </si>
+  <si>
+    <t>0141-5 | 0115-6</t>
+  </si>
+  <si>
+    <t>Produção de sementes certificadas | Cultivo de soja</t>
   </si>
 </sst>
 </file>
@@ -14361,8 +14367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1234"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16116,10 +16122,10 @@
         <v>408</v>
       </c>
       <c r="C103" t="s">
-        <v>190</v>
+        <v>4667</v>
       </c>
       <c r="D103" t="s">
-        <v>191</v>
+        <v>4668</v>
       </c>
       <c r="E103" t="s">
         <v>409</v>

</xml_diff>